<commit_message>
Added functionality to load youtube and play video till the end
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="219" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="308"/>
   </bookViews>
   <sheets>
     <sheet name="AppData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>TestName</t>
   </si>
@@ -72,17 +72,35 @@
     <t>pass</t>
   </si>
   <si>
-    <t>http://www.cleartrip.com/</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>https://youtu.be/YFoHX-yJAFM</t>
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>sc3</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>PageValidationString</t>
+  </si>
+  <si>
+    <t>YouTube</t>
+  </si>
+  <si>
+    <t>AppName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,6 +125,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -122,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -317,11 +342,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,8 +414,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,18 +783,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.5" thickBot="1">
+    <row r="1" spans="1:4" ht="13.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,128 +805,154 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="17"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="17"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4"/>
       <c r="B6" s="17"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="17"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="4"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="17"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="4"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="17"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="17"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="17"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="4"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="17"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="4"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" s="17"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="4"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="4"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="4"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="4"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="4"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="17"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="4"/>
       <c r="B19" s="17"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="4"/>
       <c r="B20" s="17"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="13.5" thickBot="1">
+      <c r="C20" s="17"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" ht="13.5" thickBot="1">
       <c r="A21" s="6"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -858,10 +962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -869,10 +973,11 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -882,11 +987,14 @@
       <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -894,13 +1002,14 @@
         <v>13</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -908,181 +1017,225 @@
         <v>16</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="24"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="24"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="24"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="24"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="24"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="24"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="24"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="24"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="24"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="24"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="24"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="24"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="24"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="24"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="24"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="24"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="24"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="24"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="24"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="24"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="24"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="24"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="24"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="24"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="24"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="24"/>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="6"/>
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
-      <c r="D31" s="7"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="7"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D31">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">

</xml_diff>

<commit_message>
Framework changes and function modifications
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>TestName</t>
   </si>
@@ -786,7 +786,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -829,6 +829,9 @@
       </c>
       <c r="B3" t="s">
         <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Modifications to execute scenarios in loop
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="308" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>TestName</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>AppName</t>
+  </si>
+  <si>
+    <t>Iteration</t>
   </si>
 </sst>
 </file>
@@ -783,21 +786,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" thickBot="1">
+    <row r="1" spans="1:5" ht="13.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,8 +814,11 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -821,9 +828,9 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -833,122 +840,143 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="4"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="17"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="17"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="4"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="17"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="4"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="17"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="17"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="4"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="17"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="4"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="17"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="4"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="17"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="4"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="17"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="4"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="17"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="4"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="17"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="4"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="17"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="4"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="17"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="4"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="17"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="4"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="17"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="4"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" ht="13.5" thickBot="1">
+      <c r="D20" s="17"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="13.5" thickBot="1">
       <c r="A21" s="6"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
-      <c r="D21" s="7"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -967,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1001,7 +1029,7 @@
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -1010,7 +1038,9 @@
       <c r="D2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">

</xml_diff>

<commit_message>
Successful implementation of dynamic method call based on keyword name at Package Level
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>TestName</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Iteration</t>
+  </si>
+  <si>
+    <t>testcase3</t>
+  </si>
+  <si>
+    <t>YMO</t>
+  </si>
+  <si>
+    <t>http://www.yourmealsonline.co.uk</t>
   </si>
 </sst>
 </file>
@@ -392,7 +401,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +432,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -789,13 +799,13 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -860,10 +870,18 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
@@ -981,9 +999,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -996,7 +1015,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1039,7 +1058,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1065,7 +1084,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Successful implementation of dynamic method call based on keyword name at Package Level and new scenario implementation
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="308" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>TestName</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>http://www.yourmealsonline.co.uk</t>
+  </si>
+  <si>
+    <t>sc4</t>
+  </si>
+  <si>
+    <t>navigateToYMORegistrationPage</t>
   </si>
 </sst>
 </file>
@@ -798,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1014,14 +1020,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1094,11 +1100,21 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="14"/>
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11"/>
@@ -1284,12 +1300,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
JSON CREATION code from YMO dropdown - interim stage
</commit_message>
<xml_diff>
--- a/ExternalData/TestData.xlsx
+++ b/ExternalData/TestData.xlsx
@@ -60,9 +60,6 @@
     <t>Navigate</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>sc2</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>sc4</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
   <si>
     <t>navigateToYMORegistrationPage</t>
@@ -825,13 +825,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -839,10 +839,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -851,10 +851,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>5</v>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1047,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1058,70 +1058,70 @@
         <v>13</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>22</v>
-      </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="14"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11"/>

</xml_diff>